<commit_message>
update for h0 calibration
the file
hng_opti_Q_optionprice_scaling_h0_calibrate_final
contains now all code for ho and no ho optimization
the file
hng_opti_Q_optionprice_scaling_h0_realVola_final
only contains the latter.
</commit_message>
<xml_diff>
--- a/Code/Calibration Calloption/szenariolist.xlsx
+++ b/Code/Calibration Calloption/szenariolist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henrik\Documents\GitHub\MasterThesisHNGDeepVola\Code\Calibration Calloption\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFDE4CCA-E7E7-48D9-AC11-F74292AEB66F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E152333-DDFC-4D85-804A-31185E9C1398}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9060" yWindow="2355" windowWidth="14385" windowHeight="11400" xr2:uid="{5EF3AB18-6B4A-4A20-80B7-077699C22F6C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5EF3AB18-6B4A-4A20-80B7-077699C22F6C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
   <si>
     <t>optll</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>done</t>
+  </si>
+  <si>
+    <t>ongoing</t>
   </si>
 </sst>
 </file>
@@ -92,9 +95,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,180 +416,223 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C644853-D4AB-442F-AC6C-55E47ADFC711}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G2" t="s">
         <v>0</v>
       </c>
-      <c r="H1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="H2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>2010</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>2010</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2011</v>
-      </c>
-      <c r="C3">
+        <v>2010</v>
+      </c>
+      <c r="B3">
         <v>1</v>
       </c>
       <c r="F3">
-        <v>2011</v>
+        <v>2010</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2012</v>
-      </c>
-      <c r="C4">
+        <v>2011</v>
+      </c>
+      <c r="B4">
         <v>1</v>
       </c>
       <c r="F4">
-        <v>2012</v>
+        <v>2011</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2013</v>
-      </c>
-      <c r="C5">
+        <v>2012</v>
+      </c>
+      <c r="B5">
         <v>1</v>
       </c>
       <c r="F5">
-        <v>2013</v>
+        <v>2012</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2014</v>
-      </c>
-      <c r="C6">
+        <v>2013</v>
+      </c>
+      <c r="B6">
         <v>1</v>
       </c>
       <c r="F6">
-        <v>2014</v>
+        <v>2013</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2015</v>
-      </c>
-      <c r="C7">
+        <v>2014</v>
+      </c>
+      <c r="B7">
         <v>1</v>
       </c>
       <c r="F7">
-        <v>2015</v>
+        <v>2014</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2016</v>
-      </c>
-      <c r="C8">
+        <v>2015</v>
+      </c>
+      <c r="B8">
         <v>1</v>
       </c>
       <c r="F8">
-        <v>2016</v>
+        <v>2015</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>2017</v>
-      </c>
-      <c r="C9">
+        <v>2016</v>
+      </c>
+      <c r="B9">
         <v>1</v>
       </c>
       <c r="F9">
-        <v>2017</v>
+        <v>2016</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
+        <v>2017</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>2017</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>2018</v>
       </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="F10">
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="F11">
         <v>2018</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="H11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>4</v>
       </c>
-      <c r="B13">
-        <f>SUM(B2:D10)</f>
+      <c r="B14">
+        <f>SUM(B3:D11)</f>
         <v>9</v>
       </c>
-      <c r="C13">
+      <c r="C14">
         <v>27</v>
       </c>
-      <c r="D13" s="1">
-        <f>B13/C13</f>
+      <c r="D14" s="1">
+        <f>B14/C14</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F14" t="s">
         <v>5</v>
       </c>
-      <c r="G13">
-        <f>SUM(G2:I10)</f>
-        <v>0</v>
-      </c>
-      <c r="H13">
+      <c r="G14">
+        <f>SUM(G3:I11)</f>
+        <v>9</v>
+      </c>
+      <c r="H14">
         <v>27</v>
       </c>
-      <c r="I13" s="1">
-        <f>G13/H13</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="I14" s="1">
+        <f>G14/H14</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>3</v>
       </c>
-      <c r="B15">
-        <f>B13+G13</f>
-        <v>9</v>
-      </c>
-      <c r="C15">
+      <c r="B16">
+        <f>B14+G14</f>
+        <v>18</v>
+      </c>
+      <c r="C16">
         <v>27</v>
       </c>
-      <c r="D15" s="1">
-        <f>B15/C15</f>
-        <v>0.33333333333333331</v>
+      <c r="D16" s="1">
+        <f>B16/C16</f>
+        <v>0.66666666666666663</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="G1:I1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
minor change in optimazation parameters
</commit_message>
<xml_diff>
--- a/Code/Calibration Calloption/szenariolist.xlsx
+++ b/Code/Calibration Calloption/szenariolist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henrik\Documents\GitHub\MasterThesisHNGDeepVola\Code\Calibration Calloption\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E152333-DDFC-4D85-804A-31185E9C1398}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87776A67-AED7-4ADF-A359-ABF667513131}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5EF3AB18-6B4A-4A20-80B7-077699C22F6C}"/>
   </bookViews>
@@ -419,7 +419,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -460,7 +460,7 @@
       <c r="A3">
         <v>2010</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>1</v>
       </c>
       <c r="F3">
@@ -474,112 +474,88 @@
       <c r="A4">
         <v>2011</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>1</v>
       </c>
       <c r="F4">
         <v>2011</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2012</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>1</v>
       </c>
       <c r="F5">
         <v>2012</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2013</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>1</v>
       </c>
       <c r="F6">
         <v>2013</v>
-      </c>
-      <c r="H6">
-        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2014</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <v>1</v>
       </c>
       <c r="F7">
         <v>2014</v>
-      </c>
-      <c r="H7">
-        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2015</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <v>1</v>
       </c>
       <c r="F8">
         <v>2015</v>
-      </c>
-      <c r="H8">
-        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2016</v>
       </c>
-      <c r="B9">
+      <c r="C9">
         <v>1</v>
       </c>
       <c r="F9">
         <v>2016</v>
-      </c>
-      <c r="H9">
-        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2017</v>
       </c>
-      <c r="B10">
+      <c r="C10">
         <v>1</v>
       </c>
       <c r="F10">
         <v>2017</v>
-      </c>
-      <c r="H10">
-        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2018</v>
       </c>
-      <c r="B11">
+      <c r="C11">
         <v>1</v>
       </c>
       <c r="F11">
         <v>2018</v>
-      </c>
-      <c r="H11">
-        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -591,25 +567,25 @@
         <v>9</v>
       </c>
       <c r="C14">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="D14" s="1">
         <f>B14/C14</f>
-        <v>0.33333333333333331</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="F14" t="s">
         <v>5</v>
       </c>
       <c r="G14">
         <f>SUM(G3:I11)</f>
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="H14">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="I14" s="1">
         <f>G14/H14</f>
-        <v>0.33333333333333331</v>
+        <v>1.8518518518518517E-2</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -618,14 +594,15 @@
       </c>
       <c r="B16">
         <f>B14+G14</f>
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C16">
-        <v>27</v>
+        <f>SUM(C14,H14)</f>
+        <v>108</v>
       </c>
       <c r="D16" s="1">
         <f>B16/C16</f>
-        <v>0.66666666666666663</v>
+        <v>9.2592592592592587E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated list of szenarios run atm
</commit_message>
<xml_diff>
--- a/Code/Calibration Calloption/szenariolist.xlsx
+++ b/Code/Calibration Calloption/szenariolist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henrik\Documents\GitHub\MasterThesisHNGDeepVola\Code\Calibration Calloption\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87776A67-AED7-4ADF-A359-ABF667513131}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F09165F4-5EBA-4C11-9462-237F15089538}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5EF3AB18-6B4A-4A20-80B7-077699C22F6C}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="9">
   <si>
     <t>optll</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>ongoing</t>
+  </si>
+  <si>
+    <t>realvol</t>
+  </si>
+  <si>
+    <t>h0cal</t>
   </si>
 </sst>
 </file>
@@ -82,7 +88,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -90,17 +96,112 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,199 +517,430 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C644853-D4AB-442F-AC6C-55E47ADFC711}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="G1" s="2" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="E2" s="2"/>
+      <c r="F2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="I2" s="2"/>
+      <c r="J2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="M2" s="2"/>
+      <c r="N2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="11">
         <v>2010</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="F3">
+      <c r="B3" s="5">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5">
+        <v>1</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="11">
         <v>2010</v>
       </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="11">
+        <v>2010</v>
+      </c>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="11">
+        <v>2010</v>
+      </c>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="6"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="11">
         <v>2011</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="F4">
+      <c r="B4" s="5"/>
+      <c r="C4" s="5">
+        <v>1</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="11">
         <v>2011</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="11">
+        <v>2011</v>
+      </c>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="11">
+        <v>2011</v>
+      </c>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="6"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="11">
         <v>2012</v>
       </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="F5">
+      <c r="B5" s="5"/>
+      <c r="C5" s="5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="11">
         <v>2012</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="11">
+        <v>2012</v>
+      </c>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="11">
+        <v>2012</v>
+      </c>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="6"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="11">
         <v>2013</v>
       </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="F6">
+      <c r="B6" s="5"/>
+      <c r="C6" s="5">
+        <v>1</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="11">
         <v>2013</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="11">
+        <v>2013</v>
+      </c>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="11">
+        <v>2013</v>
+      </c>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="6"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="11">
         <v>2014</v>
       </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="F7">
+      <c r="B7" s="5"/>
+      <c r="C7" s="5">
+        <v>1</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="11">
         <v>2014</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="11">
+        <v>2014</v>
+      </c>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="11">
+        <v>2014</v>
+      </c>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="6"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="11">
         <v>2015</v>
       </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="F8">
+      <c r="B8" s="5"/>
+      <c r="C8" s="5">
+        <v>1</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="11">
         <v>2015</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="11">
+        <v>2015</v>
+      </c>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="11">
+        <v>2015</v>
+      </c>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="6"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="11">
         <v>2016</v>
       </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="F9">
+      <c r="B9" s="5"/>
+      <c r="C9" s="5">
+        <v>1</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="11">
         <v>2016</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="11">
+        <v>2016</v>
+      </c>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="11">
+        <v>2016</v>
+      </c>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="6"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="11">
         <v>2017</v>
       </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="F10">
+      <c r="B10" s="5"/>
+      <c r="C10" s="5">
+        <v>1</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="11">
         <v>2017</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="11">
+        <v>2017</v>
+      </c>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="11">
+        <v>2017</v>
+      </c>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="6"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="12">
         <v>2018</v>
       </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="F11">
+      <c r="B11" s="7"/>
+      <c r="C11" s="7">
+        <v>1</v>
+      </c>
+      <c r="D11" s="8"/>
+      <c r="E11" s="12">
         <v>2018</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="12">
+        <v>2018</v>
+      </c>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="12">
+        <v>2018</v>
+      </c>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="8"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>4</v>
       </c>
       <c r="B14">
         <f>SUM(B3:D11)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C14">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="D14" s="1">
         <f>B14/C14</f>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="F14" t="s">
+        <v>0.37037037037037035</v>
+      </c>
+      <c r="E14" t="s">
         <v>5</v>
       </c>
+      <c r="F14">
+        <f>SUM(F3:H11)</f>
+        <v>0</v>
+      </c>
       <c r="G14">
-        <f>SUM(G3:I11)</f>
-        <v>1</v>
-      </c>
-      <c r="H14">
-        <v>54</v>
-      </c>
-      <c r="I14" s="1">
-        <f>G14/H14</f>
-        <v>1.8518518518518517E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="H14" s="1">
+        <f>F14/G14</f>
+        <v>0</v>
+      </c>
+      <c r="I14" t="s">
+        <v>4</v>
+      </c>
+      <c r="J14">
+        <f>SUM(J3:L11)</f>
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>27</v>
+      </c>
+      <c r="L14" s="1">
+        <f>J14/K14</f>
+        <v>0</v>
+      </c>
+      <c r="M14" t="s">
+        <v>5</v>
+      </c>
+      <c r="N14">
+        <f>SUM(N3:P11)</f>
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>27</v>
+      </c>
+      <c r="P14" s="1">
+        <f>N14/O14</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>3</v>
       </c>
       <c r="B16">
-        <f>B14+G14</f>
-        <v>10</v>
+        <f>N14+F14</f>
+        <v>0</v>
       </c>
       <c r="C16">
-        <f>SUM(C14,H14)</f>
-        <v>108</v>
+        <f>SUM(O14,G14)</f>
+        <v>54</v>
       </c>
       <c r="D16" s="1">
         <f>B16/C16</f>
-        <v>9.2592592592592587E-2</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="L16" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="8">
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="M1:M2"/>
     <mergeCell ref="B1:D1"/>
-    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added info in xls
added info in xls
</commit_message>
<xml_diff>
--- a/Code/Calibration Calloption/szenariolist.xlsx
+++ b/Code/Calibration Calloption/szenariolist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henrik\Documents\GitHub\MasterThesisHNGDeepVola\Code\Calibration Calloption\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lyudmila/Dropbox/GIT/HenrikAlexJP/Code/Calibration Calloption/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D25609AF-725B-4524-8BF8-18078EE2A433}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B9287AD-9048-F24F-83A2-6558464B3B43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9060" yWindow="2355" windowWidth="14385" windowHeight="11400" xr2:uid="{5EF3AB18-6B4A-4A20-80B7-077699C22F6C}"/>
+    <workbookView xWindow="9060" yWindow="2360" windowWidth="26920" windowHeight="20320" xr2:uid="{5EF3AB18-6B4A-4A20-80B7-077699C22F6C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="11">
   <si>
     <t>optll</t>
   </si>
@@ -58,6 +60,12 @@
   </si>
   <si>
     <t>h0cal</t>
+  </si>
+  <si>
+    <t>h0=ht MLE P</t>
+  </si>
+  <si>
+    <t>h0=uncond</t>
   </si>
 </sst>
 </file>
@@ -206,7 +214,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -518,15 +526,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C644853-D4AB-442F-AC6C-55E47ADFC711}">
-  <dimension ref="A1:P16"/>
+  <dimension ref="A1:P30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" customWidth="1"/>
+    <col min="9" max="9" width="11.1640625" customWidth="1"/>
+    <col min="13" max="13" width="10.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>8</v>
       </c>
@@ -560,7 +574,7 @@
       <c r="O1" s="13"/>
       <c r="P1" s="13"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="11"/>
       <c r="B2" s="7" t="s">
         <v>0</v>
@@ -602,7 +616,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="8">
         <v>2010</v>
       </c>
@@ -638,7 +652,7 @@
       <c r="O3" s="3"/>
       <c r="P3" s="4"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="8">
         <v>2011</v>
       </c>
@@ -674,7 +688,7 @@
       <c r="O4" s="3"/>
       <c r="P4" s="4"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="8">
         <v>2012</v>
       </c>
@@ -710,7 +724,7 @@
       <c r="O5" s="3"/>
       <c r="P5" s="4"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="8">
         <v>2013</v>
       </c>
@@ -746,7 +760,7 @@
       <c r="O6" s="3"/>
       <c r="P6" s="4"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="8">
         <v>2014</v>
       </c>
@@ -782,7 +796,7 @@
       <c r="O7" s="3"/>
       <c r="P7" s="4"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="8">
         <v>2015</v>
       </c>
@@ -816,7 +830,7 @@
       <c r="O8" s="3"/>
       <c r="P8" s="4"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="8">
         <v>2016</v>
       </c>
@@ -848,7 +862,7 @@
       <c r="O9" s="3"/>
       <c r="P9" s="4"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="8">
         <v>2017</v>
       </c>
@@ -880,7 +894,7 @@
       <c r="O10" s="3"/>
       <c r="P10" s="4"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="9">
         <v>2018</v>
       </c>
@@ -912,7 +926,7 @@
       <c r="O11" s="5"/>
       <c r="P11" s="6"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -970,7 +984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -988,8 +1002,328 @@
       </c>
       <c r="L16" s="1"/>
     </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A20" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J20" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="N20" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="O20" s="13"/>
+      <c r="P20" s="13"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A21" s="11"/>
+      <c r="B21" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21" s="11"/>
+      <c r="F21" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I21" s="11"/>
+      <c r="J21" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M21" s="11"/>
+      <c r="N21" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="O21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="P21" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A22" s="8">
+        <v>2010</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3">
+        <v>1</v>
+      </c>
+      <c r="D22" s="4"/>
+      <c r="E22" s="8">
+        <v>2010</v>
+      </c>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="8">
+        <v>2010</v>
+      </c>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="8">
+        <v>2010</v>
+      </c>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="4"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A23" s="8">
+        <v>2011</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="8">
+        <v>2011</v>
+      </c>
+      <c r="F23" s="3"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="8">
+        <v>2011</v>
+      </c>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="8">
+        <v>2011</v>
+      </c>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="4"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A24" s="8">
+        <v>2012</v>
+      </c>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="8">
+        <v>2012</v>
+      </c>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="8">
+        <v>2012</v>
+      </c>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="8">
+        <v>2012</v>
+      </c>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="4"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A25" s="8">
+        <v>2013</v>
+      </c>
+      <c r="B25" s="10"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="8">
+        <v>2013</v>
+      </c>
+      <c r="F25" s="3"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="8">
+        <v>2013</v>
+      </c>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="8">
+        <v>2013</v>
+      </c>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="4"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A26" s="8">
+        <v>2014</v>
+      </c>
+      <c r="B26" s="10"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="8">
+        <v>2014</v>
+      </c>
+      <c r="F26" s="3"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="8">
+        <v>2014</v>
+      </c>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="8">
+        <v>2014</v>
+      </c>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="4"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A27" s="8">
+        <v>2015</v>
+      </c>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="8">
+        <v>2015</v>
+      </c>
+      <c r="F27" s="3"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="8">
+        <v>2015</v>
+      </c>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="8">
+        <v>2015</v>
+      </c>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+      <c r="P27" s="4"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A28" s="8">
+        <v>2016</v>
+      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="8">
+        <v>2016</v>
+      </c>
+      <c r="F28" s="3"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="8">
+        <v>2016</v>
+      </c>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="8">
+        <v>2016</v>
+      </c>
+      <c r="N28" s="3"/>
+      <c r="O28" s="3"/>
+      <c r="P28" s="4"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A29" s="8">
+        <v>2017</v>
+      </c>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="8">
+        <v>2017</v>
+      </c>
+      <c r="F29" s="3"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="8">
+        <v>2017</v>
+      </c>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="4"/>
+      <c r="M29" s="8">
+        <v>2017</v>
+      </c>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3"/>
+      <c r="P29" s="4"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A30" s="9">
+        <v>2018</v>
+      </c>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="9">
+        <v>2018</v>
+      </c>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="9">
+        <v>2018</v>
+      </c>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="6"/>
+      <c r="M30" s="9">
+        <v>2018</v>
+      </c>
+      <c r="N30" s="5"/>
+      <c r="O30" s="5"/>
+      <c r="P30" s="6"/>
+    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="16">
+    <mergeCell ref="J20:L20"/>
+    <mergeCell ref="M20:M21"/>
+    <mergeCell ref="N20:P20"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="I20:I21"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="J1:L1"/>

</xml_diff>

<commit_message>
server merge and shift of the mle calibration tothe mainfile
</commit_message>
<xml_diff>
--- a/Code/Calibration Calloption/szenariolist.xlsx
+++ b/Code/Calibration Calloption/szenariolist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lyudmila/Dropbox/GIT/HenrikAlexJP/Code/Calibration Calloption/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henrik\Documents\GitHub\MasterThesisHNGDeepVola\Code\Calibration Calloption\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B9287AD-9048-F24F-83A2-6558464B3B43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F46032E4-2A02-4EC4-800D-DA6C12798FF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9060" yWindow="2360" windowWidth="26920" windowHeight="20320" xr2:uid="{5EF3AB18-6B4A-4A20-80B7-077699C22F6C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5EF3AB18-6B4A-4A20-80B7-077699C22F6C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -202,19 +200,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -529,53 +527,53 @@
   <dimension ref="A1:P30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" customWidth="1"/>
-    <col min="9" max="9" width="11.1640625" customWidth="1"/>
-    <col min="13" max="13" width="10.83203125" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="11" t="s">
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="11" t="s">
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="11" t="s">
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="N1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A2" s="11"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="13"/>
       <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
@@ -585,7 +583,7 @@
       <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="11"/>
+      <c r="E2" s="13"/>
       <c r="F2" s="7" t="s">
         <v>0</v>
       </c>
@@ -595,7 +593,7 @@
       <c r="H2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="11"/>
+      <c r="I2" s="13"/>
       <c r="J2" s="7" t="s">
         <v>0</v>
       </c>
@@ -605,7 +603,7 @@
       <c r="L2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="M2" s="11"/>
+      <c r="M2" s="13"/>
       <c r="N2" s="7" t="s">
         <v>0</v>
       </c>
@@ -616,14 +614,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>2010</v>
       </c>
-      <c r="B3" s="3">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3">
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
         <v>0</v>
       </c>
       <c r="D3" s="4">
@@ -632,8 +630,10 @@
       <c r="E3" s="8">
         <v>2010</v>
       </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3">
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
         <v>1</v>
       </c>
       <c r="H3" s="4">
@@ -652,14 +652,14 @@
       <c r="O3" s="3"/>
       <c r="P3" s="4"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>2011</v>
       </c>
-      <c r="B4" s="3">
-        <v>1</v>
-      </c>
-      <c r="C4" s="3">
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
         <v>0</v>
       </c>
       <c r="D4" s="4">
@@ -668,8 +668,10 @@
       <c r="E4" s="8">
         <v>2011</v>
       </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="10">
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
         <v>1</v>
       </c>
       <c r="H4" s="4">
@@ -688,14 +690,14 @@
       <c r="O4" s="3"/>
       <c r="P4" s="4"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>2012</v>
       </c>
-      <c r="B5" s="3">
-        <v>1</v>
-      </c>
-      <c r="C5" s="3">
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
         <v>0</v>
       </c>
       <c r="D5" s="4">
@@ -704,8 +706,10 @@
       <c r="E5" s="8">
         <v>2012</v>
       </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3">
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
         <v>1</v>
       </c>
       <c r="H5" s="4">
@@ -724,14 +728,14 @@
       <c r="O5" s="3"/>
       <c r="P5" s="4"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>2013</v>
       </c>
-      <c r="B6" s="10">
-        <v>1</v>
-      </c>
-      <c r="C6" s="3">
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
         <v>0</v>
       </c>
       <c r="D6" s="4">
@@ -740,8 +744,10 @@
       <c r="E6" s="8">
         <v>2013</v>
       </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="10">
+      <c r="F6" s="10">
+        <v>1</v>
+      </c>
+      <c r="G6">
         <v>1</v>
       </c>
       <c r="H6" s="4">
@@ -760,14 +766,14 @@
       <c r="O6" s="3"/>
       <c r="P6" s="4"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>2014</v>
       </c>
-      <c r="B7" s="10">
-        <v>1</v>
-      </c>
-      <c r="C7" s="3">
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
         <v>0</v>
       </c>
       <c r="D7" s="4">
@@ -776,8 +782,10 @@
       <c r="E7" s="8">
         <v>2014</v>
       </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="10">
+      <c r="F7" s="10">
+        <v>1</v>
+      </c>
+      <c r="G7">
         <v>1</v>
       </c>
       <c r="H7" s="4">
@@ -796,27 +804,31 @@
       <c r="O7" s="3"/>
       <c r="P7" s="4"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>2015</v>
       </c>
-      <c r="B8" s="10">
-        <v>1</v>
-      </c>
-      <c r="C8" s="10">
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
         <v>0</v>
       </c>
       <c r="D8" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" s="8">
         <v>2015</v>
       </c>
-      <c r="F8" s="3"/>
-      <c r="G8" s="10">
-        <v>1</v>
-      </c>
-      <c r="H8" s="4"/>
+      <c r="F8" s="10">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8" s="4">
+        <v>1</v>
+      </c>
       <c r="I8" s="8">
         <v>2015</v>
       </c>
@@ -830,25 +842,28 @@
       <c r="O8" s="3"/>
       <c r="P8" s="4"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>2016</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3">
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
         <v>0</v>
       </c>
       <c r="D9" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" s="8">
         <v>2016</v>
       </c>
-      <c r="F9" s="3"/>
-      <c r="G9" s="10">
-        <v>1</v>
-      </c>
-      <c r="H9" s="4"/>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9" s="4">
+        <v>1</v>
+      </c>
       <c r="I9" s="8">
         <v>2016</v>
       </c>
@@ -862,25 +877,28 @@
       <c r="O9" s="3"/>
       <c r="P9" s="4"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>2017</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3">
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
         <v>0</v>
       </c>
       <c r="D10" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10" s="8">
         <v>2017</v>
       </c>
-      <c r="F10" s="3"/>
-      <c r="G10" s="10">
-        <v>1</v>
-      </c>
-      <c r="H10" s="4"/>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10" s="4">
+        <v>1</v>
+      </c>
       <c r="I10" s="8">
         <v>2017</v>
       </c>
@@ -894,16 +912,18 @@
       <c r="O10" s="3"/>
       <c r="P10" s="4"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>2018</v>
       </c>
-      <c r="B11" s="5"/>
+      <c r="B11" s="5">
+        <v>1</v>
+      </c>
       <c r="C11" s="5">
         <v>0</v>
       </c>
       <c r="D11" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" s="9">
         <v>2018</v>
@@ -912,7 +932,9 @@
       <c r="G11" s="5">
         <v>1</v>
       </c>
-      <c r="H11" s="6"/>
+      <c r="H11" s="6">
+        <v>1</v>
+      </c>
       <c r="I11" s="9">
         <v>2018</v>
       </c>
@@ -926,34 +948,34 @@
       <c r="O11" s="5"/>
       <c r="P11" s="6"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>4</v>
       </c>
       <c r="B14">
         <f>SUM(B3:D11)</f>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C14">
         <v>27</v>
       </c>
       <c r="D14" s="1">
         <f>B14/C14</f>
-        <v>0.37037037037037035</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="E14" t="s">
         <v>5</v>
       </c>
       <c r="F14">
         <f>SUM(F3:H11)</f>
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="G14">
         <v>27</v>
       </c>
       <c r="H14" s="1">
         <f>F14/G14</f>
-        <v>0.51851851851851849</v>
+        <v>0.88888888888888884</v>
       </c>
       <c r="I14" t="s">
         <v>4</v>
@@ -984,13 +1006,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>3</v>
       </c>
       <c r="B16">
         <f>N14+F14</f>
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="C16">
         <f>SUM(O14,G14)</f>
@@ -998,46 +1020,46 @@
       </c>
       <c r="D16" s="1">
         <f>B16/C16</f>
-        <v>0.25925925925925924</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="L16" s="1"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A20" s="11" t="s">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="11" t="s">
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F20" s="12" t="s">
+      <c r="F20" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="11" t="s">
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="J20" s="12" t="s">
+      <c r="J20" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="11" t="s">
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="N20" s="12" t="s">
+      <c r="N20" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="O20" s="13"/>
-      <c r="P20" s="13"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A21" s="11"/>
+      <c r="O20" s="12"/>
+      <c r="P20" s="12"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21" s="13"/>
       <c r="B21" s="7" t="s">
         <v>0</v>
       </c>
@@ -1047,7 +1069,7 @@
       <c r="D21" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E21" s="11"/>
+      <c r="E21" s="13"/>
       <c r="F21" s="7" t="s">
         <v>0</v>
       </c>
@@ -1057,7 +1079,7 @@
       <c r="H21" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I21" s="11"/>
+      <c r="I21" s="13"/>
       <c r="J21" s="7" t="s">
         <v>0</v>
       </c>
@@ -1067,7 +1089,7 @@
       <c r="L21" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="M21" s="11"/>
+      <c r="M21" s="13"/>
       <c r="N21" s="7" t="s">
         <v>0</v>
       </c>
@@ -1078,7 +1100,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <v>2010</v>
       </c>
@@ -1106,7 +1128,7 @@
       <c r="O22" s="3"/>
       <c r="P22" s="4"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <v>2011</v>
       </c>
@@ -1132,7 +1154,7 @@
       <c r="O23" s="3"/>
       <c r="P23" s="4"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <v>2012</v>
       </c>
@@ -1158,7 +1180,7 @@
       <c r="O24" s="3"/>
       <c r="P24" s="4"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <v>2013</v>
       </c>
@@ -1184,7 +1206,7 @@
       <c r="O25" s="3"/>
       <c r="P25" s="4"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="8">
         <v>2014</v>
       </c>
@@ -1210,7 +1232,7 @@
       <c r="O26" s="3"/>
       <c r="P26" s="4"/>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="8">
         <v>2015</v>
       </c>
@@ -1236,7 +1258,7 @@
       <c r="O27" s="3"/>
       <c r="P27" s="4"/>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
         <v>2016</v>
       </c>
@@ -1262,7 +1284,7 @@
       <c r="O28" s="3"/>
       <c r="P28" s="4"/>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="8">
         <v>2017</v>
       </c>
@@ -1288,7 +1310,7 @@
       <c r="O29" s="3"/>
       <c r="P29" s="4"/>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="9">
         <v>2018</v>
       </c>
@@ -1316,6 +1338,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="F1:H1"/>
     <mergeCell ref="J20:L20"/>
     <mergeCell ref="M20:M21"/>
     <mergeCell ref="N20:P20"/>
@@ -1324,14 +1354,6 @@
     <mergeCell ref="E20:E21"/>
     <mergeCell ref="F20:H20"/>
     <mergeCell ref="I20:I21"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="N1:P1"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="F1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated status in excel sheet
</commit_message>
<xml_diff>
--- a/Code/Calibration Calloption/szenariolist.xlsx
+++ b/Code/Calibration Calloption/szenariolist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lyudmila/Dropbox/GIT/HenrikAlexJP/Code/Calibration Calloption/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{557CB99E-676C-3C4E-825D-1ED29238D745}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B26E498-F003-F749-92D4-5620EC3B5344}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-220" yWindow="460" windowWidth="35680" windowHeight="21160" xr2:uid="{5EF3AB18-6B4A-4A20-80B7-077699C22F6C}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35680" windowHeight="21160" xr2:uid="{5EF3AB18-6B4A-4A20-80B7-077699C22F6C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -202,14 +202,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -529,7 +529,7 @@
   <dimension ref="A1:P30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -541,41 +541,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="11" t="s">
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="11" t="s">
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="11" t="s">
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="N1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A2" s="11"/>
+      <c r="A2" s="13"/>
       <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
@@ -585,7 +585,7 @@
       <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="11"/>
+      <c r="E2" s="13"/>
       <c r="F2" s="7" t="s">
         <v>0</v>
       </c>
@@ -595,7 +595,7 @@
       <c r="H2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="11"/>
+      <c r="I2" s="13"/>
       <c r="J2" s="7" t="s">
         <v>0</v>
       </c>
@@ -605,7 +605,7 @@
       <c r="L2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="M2" s="11"/>
+      <c r="M2" s="13"/>
       <c r="N2" s="7" t="s">
         <v>0</v>
       </c>
@@ -1035,41 +1035,41 @@
       <c r="L16" s="1"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="11" t="s">
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F20" s="12" t="s">
+      <c r="F20" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="11" t="s">
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="J20" s="12" t="s">
+      <c r="J20" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="11" t="s">
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="N20" s="12" t="s">
+      <c r="N20" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="O20" s="13"/>
-      <c r="P20" s="13"/>
+      <c r="O20" s="12"/>
+      <c r="P20" s="12"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A21" s="11"/>
+      <c r="A21" s="13"/>
       <c r="B21" s="7" t="s">
         <v>0</v>
       </c>
@@ -1079,7 +1079,7 @@
       <c r="D21" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E21" s="11"/>
+      <c r="E21" s="13"/>
       <c r="F21" s="7" t="s">
         <v>0</v>
       </c>
@@ -1089,7 +1089,7 @@
       <c r="H21" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I21" s="11"/>
+      <c r="I21" s="13"/>
       <c r="J21" s="7" t="s">
         <v>0</v>
       </c>
@@ -1099,7 +1099,7 @@
       <c r="L21" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="M21" s="11"/>
+      <c r="M21" s="13"/>
       <c r="N21" s="7" t="s">
         <v>0</v>
       </c>
@@ -1161,7 +1161,9 @@
         <v>2011</v>
       </c>
       <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
+      <c r="K23" s="3">
+        <v>1</v>
+      </c>
       <c r="L23" s="4"/>
       <c r="M23" s="8">
         <v>2011</v>
@@ -1189,7 +1191,9 @@
         <v>2012</v>
       </c>
       <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
+      <c r="K24" s="3">
+        <v>1</v>
+      </c>
       <c r="L24" s="4"/>
       <c r="M24" s="8">
         <v>2012</v>
@@ -1217,7 +1221,9 @@
         <v>2013</v>
       </c>
       <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
+      <c r="K25" s="10">
+        <v>1</v>
+      </c>
       <c r="L25" s="4"/>
       <c r="M25" s="8">
         <v>2013</v>
@@ -1231,7 +1237,9 @@
         <v>2014</v>
       </c>
       <c r="B26" s="10"/>
-      <c r="C26" s="3"/>
+      <c r="C26" s="10">
+        <v>1</v>
+      </c>
       <c r="D26" s="4"/>
       <c r="E26" s="8">
         <v>2014</v>
@@ -1243,7 +1251,9 @@
         <v>2014</v>
       </c>
       <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
+      <c r="K26" s="10">
+        <v>1</v>
+      </c>
       <c r="L26" s="4"/>
       <c r="M26" s="8">
         <v>2014</v>
@@ -1257,7 +1267,9 @@
         <v>2015</v>
       </c>
       <c r="B27" s="10"/>
-      <c r="C27" s="10"/>
+      <c r="C27" s="10">
+        <v>1</v>
+      </c>
       <c r="D27" s="4"/>
       <c r="E27" s="8">
         <v>2015</v>
@@ -1269,7 +1281,9 @@
         <v>2015</v>
       </c>
       <c r="J27" s="3"/>
-      <c r="K27" s="3"/>
+      <c r="K27" s="10">
+        <v>1</v>
+      </c>
       <c r="L27" s="4"/>
       <c r="M27" s="8">
         <v>2015</v>
@@ -1283,7 +1297,9 @@
         <v>2016</v>
       </c>
       <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
+      <c r="C28" s="10">
+        <v>1</v>
+      </c>
       <c r="D28" s="4"/>
       <c r="E28" s="8">
         <v>2016</v>
@@ -1309,7 +1325,9 @@
         <v>2017</v>
       </c>
       <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
+      <c r="C29" s="10">
+        <v>1</v>
+      </c>
       <c r="D29" s="4"/>
       <c r="E29" s="8">
         <v>2017</v>
@@ -1335,7 +1353,9 @@
         <v>2018</v>
       </c>
       <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
+      <c r="C30" s="5">
+        <v>1</v>
+      </c>
       <c r="D30" s="6"/>
       <c r="E30" s="9">
         <v>2018</v>
@@ -1358,6 +1378,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="F1:H1"/>
     <mergeCell ref="J20:L20"/>
     <mergeCell ref="M20:M21"/>
     <mergeCell ref="N20:P20"/>
@@ -1366,14 +1394,6 @@
     <mergeCell ref="E20:E21"/>
     <mergeCell ref="F20:H20"/>
     <mergeCell ref="I20:I21"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="N1:P1"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="F1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update generator and scenariolist
</commit_message>
<xml_diff>
--- a/Code/Calibration Calloption/szenariolist.xlsx
+++ b/Code/Calibration Calloption/szenariolist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lyudmila/Dropbox/GIT/HenrikAlexJP/Code/Calibration Calloption/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henrik\Documents\GitHub\MasterThesisHNGDeepVola\Code\Calibration Calloption\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75DE0DF5-1C15-FB47-AF09-529DFBE164B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3178099D-6748-4236-93C3-BB712AD31E32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39380" yWindow="460" windowWidth="35680" windowHeight="20540" xr2:uid="{5EF3AB18-6B4A-4A20-80B7-077699C22F6C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5EF3AB18-6B4A-4A20-80B7-077699C22F6C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="26">
   <si>
     <t>optll</t>
   </si>
@@ -78,6 +76,39 @@
   </si>
   <si>
     <t>with 1 starting point, h0P is taken as unconditional</t>
+  </si>
+  <si>
+    <t>Dataset Generator</t>
+  </si>
+  <si>
+    <t>uni</t>
+  </si>
+  <si>
+    <t>log</t>
+  </si>
+  <si>
+    <t>norm</t>
+  </si>
+  <si>
+    <t>tanh</t>
+  </si>
+  <si>
+    <t>tanhscale</t>
+  </si>
+  <si>
+    <t>unisemiscale</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>filter</t>
+  </si>
+  <si>
+    <t>yields</t>
+  </si>
+  <si>
+    <t>scenario</t>
   </si>
 </sst>
 </file>
@@ -258,6 +289,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -267,22 +304,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -291,7 +322,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -603,56 +634,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C644853-D4AB-442F-AC6C-55E47ADFC711}">
-  <dimension ref="A1:P59"/>
+  <dimension ref="A1:W59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="N63" sqref="N63"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V14" sqref="V14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" customWidth="1"/>
-    <col min="9" max="9" width="11.1640625" customWidth="1"/>
-    <col min="13" max="13" width="10.83203125" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="13" t="s">
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="13" t="s">
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="13" t="s">
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="11" t="s">
+      <c r="N1" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A2" s="13"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="S1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2" s="19"/>
       <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
@@ -662,7 +696,7 @@
       <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="13"/>
+      <c r="E2" s="19"/>
       <c r="F2" s="7" t="s">
         <v>0</v>
       </c>
@@ -672,7 +706,7 @@
       <c r="H2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="13"/>
+      <c r="I2" s="19"/>
       <c r="J2" s="7" t="s">
         <v>0</v>
       </c>
@@ -682,7 +716,7 @@
       <c r="L2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="M2" s="13"/>
+      <c r="M2" s="19"/>
       <c r="N2" s="7" t="s">
         <v>0</v>
       </c>
@@ -692,8 +726,23 @@
       <c r="P2" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="S2" t="s">
+        <v>22</v>
+      </c>
+      <c r="T2" t="s">
+        <v>23</v>
+      </c>
+      <c r="U2" t="s">
+        <v>24</v>
+      </c>
+      <c r="V2" t="s">
+        <v>6</v>
+      </c>
+      <c r="W2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>2010</v>
       </c>
@@ -730,8 +779,20 @@
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>
       <c r="P3" s="4"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="S3" t="s">
+        <v>16</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3" t="s">
+        <v>25</v>
+      </c>
+      <c r="W3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>2011</v>
       </c>
@@ -768,8 +829,20 @@
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
       <c r="P4" s="4"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="S4" t="s">
+        <v>17</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4" t="s">
+        <v>25</v>
+      </c>
+      <c r="W4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>2012</v>
       </c>
@@ -806,8 +879,20 @@
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
       <c r="P5" s="4"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="S5" t="s">
+        <v>18</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5" t="s">
+        <v>25</v>
+      </c>
+      <c r="W5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>2013</v>
       </c>
@@ -844,8 +929,20 @@
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
       <c r="P6" s="4"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="S6" t="s">
+        <v>19</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6" t="s">
+        <v>25</v>
+      </c>
+      <c r="W6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>2014</v>
       </c>
@@ -882,8 +979,20 @@
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
       <c r="P7" s="4"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="S7" t="s">
+        <v>20</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7" t="s">
+        <v>25</v>
+      </c>
+      <c r="W7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>2015</v>
       </c>
@@ -920,8 +1029,20 @@
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
       <c r="P8" s="4"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="S8" t="s">
+        <v>21</v>
+      </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="U8" t="s">
+        <v>25</v>
+      </c>
+      <c r="W8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>2016</v>
       </c>
@@ -958,8 +1079,20 @@
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
       <c r="P9" s="4"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="S9" t="s">
+        <v>16</v>
+      </c>
+      <c r="T9">
+        <v>1</v>
+      </c>
+      <c r="U9" t="s">
+        <v>25</v>
+      </c>
+      <c r="V9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>2017</v>
       </c>
@@ -996,8 +1129,20 @@
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
       <c r="P10" s="4"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="S10" t="s">
+        <v>17</v>
+      </c>
+      <c r="T10">
+        <v>1</v>
+      </c>
+      <c r="U10" t="s">
+        <v>25</v>
+      </c>
+      <c r="V10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>2018</v>
       </c>
@@ -1034,8 +1179,48 @@
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
       <c r="P11" s="6"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="S11" t="s">
+        <v>18</v>
+      </c>
+      <c r="T11">
+        <v>1</v>
+      </c>
+      <c r="U11" t="s">
+        <v>25</v>
+      </c>
+      <c r="V11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="S12" t="s">
+        <v>19</v>
+      </c>
+      <c r="T12">
+        <v>1</v>
+      </c>
+      <c r="U12" t="s">
+        <v>25</v>
+      </c>
+      <c r="V12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="S13" t="s">
+        <v>20</v>
+      </c>
+      <c r="T13">
+        <v>1</v>
+      </c>
+      <c r="U13" t="s">
+        <v>25</v>
+      </c>
+      <c r="V13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -1092,8 +1277,20 @@
         <f>N14/O14</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="S14" t="s">
+        <v>21</v>
+      </c>
+      <c r="T14">
+        <v>1</v>
+      </c>
+      <c r="U14" t="s">
+        <v>25</v>
+      </c>
+      <c r="V14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -1111,47 +1308,47 @@
       </c>
       <c r="L16" s="1"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A20" s="13" t="s">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="13" t="s">
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="F20" s="11" t="s">
+      <c r="F20" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="13" t="s">
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="J20" s="11" t="s">
+      <c r="J20" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="K20" s="12"/>
-      <c r="L20" s="12"/>
-      <c r="M20" s="13" t="s">
+      <c r="K20" s="18"/>
+      <c r="L20" s="18"/>
+      <c r="M20" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="N20" s="11" t="s">
+      <c r="N20" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="O20" s="12"/>
-      <c r="P20" s="12"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A21" s="13"/>
+      <c r="O20" s="18"/>
+      <c r="P20" s="18"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21" s="19"/>
       <c r="B21" s="7" t="s">
         <v>0</v>
       </c>
@@ -1161,7 +1358,7 @@
       <c r="D21" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E21" s="13"/>
+      <c r="E21" s="19"/>
       <c r="F21" s="7" t="s">
         <v>0</v>
       </c>
@@ -1171,7 +1368,7 @@
       <c r="H21" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I21" s="13"/>
+      <c r="I21" s="19"/>
       <c r="J21" s="7" t="s">
         <v>0</v>
       </c>
@@ -1181,7 +1378,7 @@
       <c r="L21" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="M21" s="13"/>
+      <c r="M21" s="19"/>
       <c r="N21" s="7" t="s">
         <v>0</v>
       </c>
@@ -1192,7 +1389,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <v>2010</v>
       </c>
@@ -1226,7 +1423,7 @@
       </c>
       <c r="P22" s="4"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <v>2011</v>
       </c>
@@ -1260,7 +1457,7 @@
       </c>
       <c r="P23" s="4"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <v>2012</v>
       </c>
@@ -1294,7 +1491,7 @@
       </c>
       <c r="P24" s="4"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <v>2013</v>
       </c>
@@ -1328,7 +1525,7 @@
       </c>
       <c r="P25" s="4"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="8">
         <v>2014</v>
       </c>
@@ -1362,7 +1559,7 @@
       </c>
       <c r="P26" s="4"/>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="8">
         <v>2015</v>
       </c>
@@ -1396,7 +1593,7 @@
       </c>
       <c r="P27" s="4"/>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
         <v>2016</v>
       </c>
@@ -1430,7 +1627,7 @@
       </c>
       <c r="P28" s="4"/>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="8">
         <v>2017</v>
       </c>
@@ -1464,7 +1661,7 @@
       </c>
       <c r="P29" s="4"/>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="9">
         <v>2018</v>
       </c>
@@ -1498,47 +1695,47 @@
       </c>
       <c r="P30" s="6"/>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A34" s="13" t="s">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A34" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B34" s="11" t="s">
+      <c r="B34" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="13" t="s">
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="F34" s="11" t="s">
+      <c r="F34" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="G34" s="12"/>
-      <c r="H34" s="12"/>
-      <c r="I34" s="13" t="s">
+      <c r="G34" s="18"/>
+      <c r="H34" s="18"/>
+      <c r="I34" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="J34" s="11" t="s">
+      <c r="J34" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="K34" s="12"/>
-      <c r="L34" s="12"/>
-      <c r="M34" s="13" t="s">
+      <c r="K34" s="18"/>
+      <c r="L34" s="18"/>
+      <c r="M34" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="N34" s="11" t="s">
+      <c r="N34" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="O34" s="12"/>
-      <c r="P34" s="12"/>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A35" s="13"/>
+      <c r="O34" s="18"/>
+      <c r="P34" s="18"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A35" s="19"/>
       <c r="B35" s="7" t="s">
         <v>0</v>
       </c>
@@ -1548,7 +1745,7 @@
       <c r="D35" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E35" s="13"/>
+      <c r="E35" s="19"/>
       <c r="F35" s="7" t="s">
         <v>0</v>
       </c>
@@ -1558,7 +1755,7 @@
       <c r="H35" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I35" s="13"/>
+      <c r="I35" s="19"/>
       <c r="J35" s="7" t="s">
         <v>0</v>
       </c>
@@ -1568,7 +1765,7 @@
       <c r="L35" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="M35" s="13"/>
+      <c r="M35" s="19"/>
       <c r="N35" s="7" t="s">
         <v>0</v>
       </c>
@@ -1579,7 +1776,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="8">
         <v>2010</v>
       </c>
@@ -1607,7 +1804,7 @@
       <c r="O36" s="3"/>
       <c r="P36" s="4"/>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="8">
         <v>2011</v>
       </c>
@@ -1633,7 +1830,7 @@
       <c r="O37" s="3"/>
       <c r="P37" s="4"/>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="8">
         <v>2012</v>
       </c>
@@ -1661,7 +1858,7 @@
       <c r="O38" s="3"/>
       <c r="P38" s="4"/>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="8">
         <v>2013</v>
       </c>
@@ -1687,7 +1884,7 @@
       <c r="O39" s="10"/>
       <c r="P39" s="4"/>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="8">
         <v>2014</v>
       </c>
@@ -1713,7 +1910,7 @@
       <c r="O40" s="10"/>
       <c r="P40" s="4"/>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="8">
         <v>2015</v>
       </c>
@@ -1739,7 +1936,7 @@
       <c r="O41" s="10"/>
       <c r="P41" s="4"/>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="8">
         <v>2016</v>
       </c>
@@ -1765,7 +1962,7 @@
       <c r="O42" s="10"/>
       <c r="P42" s="4"/>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="8">
         <v>2017</v>
       </c>
@@ -1791,7 +1988,7 @@
       <c r="O43" s="10"/>
       <c r="P43" s="4"/>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="9">
         <v>2018</v>
       </c>
@@ -1817,343 +2014,359 @@
       <c r="O44" s="5"/>
       <c r="P44" s="6"/>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A48" s="14" t="s">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A48" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B48" s="14"/>
-      <c r="C48" s="14"/>
-      <c r="D48" s="14"/>
-      <c r="E48" s="14"/>
-      <c r="F48" s="14"/>
-      <c r="G48" s="14"/>
-      <c r="H48" s="14"/>
-      <c r="I48" s="14"/>
-      <c r="J48" s="14"/>
-      <c r="K48" s="14"/>
-      <c r="L48" s="14"/>
-      <c r="M48" s="14"/>
-      <c r="N48" s="14"/>
-      <c r="O48" s="14"/>
-      <c r="P48" s="14"/>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B48" s="11"/>
+      <c r="C48" s="11"/>
+      <c r="D48" s="11"/>
+      <c r="E48" s="11"/>
+      <c r="F48" s="11"/>
+      <c r="G48" s="11"/>
+      <c r="H48" s="11"/>
+      <c r="I48" s="11"/>
+      <c r="J48" s="11"/>
+      <c r="K48" s="11"/>
+      <c r="L48" s="11"/>
+      <c r="M48" s="11"/>
+      <c r="N48" s="11"/>
+      <c r="O48" s="11"/>
+      <c r="P48" s="11"/>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B49" s="23" t="s">
+      <c r="B49" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="C49" s="22"/>
+      <c r="C49" s="23"/>
       <c r="D49" s="24"/>
       <c r="E49" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="F49" s="23" t="s">
+      <c r="F49" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="G49" s="22"/>
+      <c r="G49" s="23"/>
       <c r="H49" s="24"/>
       <c r="I49" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="J49" s="23" t="s">
+      <c r="J49" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="K49" s="22"/>
+      <c r="K49" s="23"/>
       <c r="L49" s="24"/>
       <c r="M49" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="N49" s="23" t="s">
+      <c r="N49" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="O49" s="22"/>
+      <c r="O49" s="23"/>
       <c r="P49" s="24"/>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" s="21"/>
-      <c r="B50" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C50" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="D50" s="15" t="s">
+      <c r="B50" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C50" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D50" s="12" t="s">
         <v>2</v>
       </c>
       <c r="E50" s="21"/>
-      <c r="F50" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="G50" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="H50" s="15" t="s">
+      <c r="F50" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="G50" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="H50" s="12" t="s">
         <v>2</v>
       </c>
       <c r="I50" s="21"/>
-      <c r="J50" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="K50" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="L50" s="15" t="s">
+      <c r="J50" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="K50" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="L50" s="12" t="s">
         <v>2</v>
       </c>
       <c r="M50" s="21"/>
-      <c r="N50" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="O50" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="P50" s="15" t="s">
+      <c r="N50" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="O50" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="P50" s="12" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A51" s="16">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A51" s="13">
         <v>2010</v>
       </c>
-      <c r="B51" s="14"/>
-      <c r="C51" s="14"/>
-      <c r="D51" s="17"/>
-      <c r="E51" s="17">
+      <c r="B51" s="11"/>
+      <c r="C51" s="11"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="14">
         <v>2010</v>
       </c>
-      <c r="F51" s="14"/>
-      <c r="G51" s="14"/>
-      <c r="H51" s="17"/>
-      <c r="I51" s="17">
+      <c r="F51" s="11"/>
+      <c r="G51" s="11"/>
+      <c r="H51" s="14"/>
+      <c r="I51" s="14">
         <v>2010</v>
       </c>
-      <c r="J51" s="14"/>
-      <c r="K51" s="14"/>
-      <c r="L51" s="17"/>
-      <c r="M51" s="17">
+      <c r="J51" s="11"/>
+      <c r="K51" s="11"/>
+      <c r="L51" s="14"/>
+      <c r="M51" s="14">
         <v>2010</v>
       </c>
-      <c r="N51" s="14"/>
-      <c r="O51" s="14"/>
-      <c r="P51" s="17"/>
-    </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A52" s="16">
+      <c r="N51" s="11"/>
+      <c r="O51" s="11"/>
+      <c r="P51" s="14"/>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A52" s="13">
         <v>2011</v>
       </c>
-      <c r="B52" s="14"/>
-      <c r="C52" s="14"/>
-      <c r="D52" s="17"/>
-      <c r="E52" s="17">
+      <c r="B52" s="11"/>
+      <c r="C52" s="11"/>
+      <c r="D52" s="14"/>
+      <c r="E52" s="14">
         <v>2011</v>
       </c>
-      <c r="F52" s="14"/>
-      <c r="G52" s="14"/>
-      <c r="H52" s="17"/>
-      <c r="I52" s="17">
+      <c r="F52" s="11"/>
+      <c r="G52" s="11"/>
+      <c r="H52" s="14"/>
+      <c r="I52" s="14">
         <v>2011</v>
       </c>
-      <c r="J52" s="14"/>
-      <c r="K52" s="14"/>
-      <c r="L52" s="17"/>
-      <c r="M52" s="17">
+      <c r="J52" s="11"/>
+      <c r="K52" s="11"/>
+      <c r="L52" s="14"/>
+      <c r="M52" s="14">
         <v>2011</v>
       </c>
-      <c r="N52" s="14"/>
-      <c r="O52" s="14"/>
-      <c r="P52" s="17"/>
-    </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A53" s="16">
+      <c r="N52" s="11"/>
+      <c r="O52" s="11"/>
+      <c r="P52" s="14"/>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A53" s="13">
         <v>2012</v>
       </c>
-      <c r="B53" s="14"/>
-      <c r="C53" s="14"/>
-      <c r="D53" s="17"/>
-      <c r="E53" s="17">
+      <c r="B53" s="11"/>
+      <c r="C53" s="11"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="14">
         <v>2012</v>
       </c>
-      <c r="F53" s="14"/>
-      <c r="G53" s="14"/>
-      <c r="H53" s="17"/>
-      <c r="I53" s="17">
+      <c r="F53" s="11"/>
+      <c r="G53" s="11"/>
+      <c r="H53" s="14"/>
+      <c r="I53" s="14">
         <v>2012</v>
       </c>
-      <c r="J53" s="14"/>
-      <c r="K53" s="14"/>
-      <c r="L53" s="17"/>
-      <c r="M53" s="17">
+      <c r="J53" s="11"/>
+      <c r="K53" s="11"/>
+      <c r="L53" s="14"/>
+      <c r="M53" s="14">
         <v>2012</v>
       </c>
-      <c r="N53" s="14"/>
-      <c r="O53" s="14"/>
-      <c r="P53" s="17"/>
-    </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A54" s="16">
+      <c r="N53" s="11"/>
+      <c r="O53" s="11"/>
+      <c r="P53" s="14"/>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A54" s="13">
         <v>2013</v>
       </c>
-      <c r="B54" s="14"/>
-      <c r="C54" s="14"/>
-      <c r="D54" s="17"/>
-      <c r="E54" s="17">
+      <c r="B54" s="11"/>
+      <c r="C54" s="11"/>
+      <c r="D54" s="14"/>
+      <c r="E54" s="14">
         <v>2013</v>
       </c>
-      <c r="F54" s="14"/>
-      <c r="G54" s="14"/>
-      <c r="H54" s="17"/>
-      <c r="I54" s="17">
+      <c r="F54" s="11"/>
+      <c r="G54" s="11"/>
+      <c r="H54" s="14"/>
+      <c r="I54" s="14">
         <v>2013</v>
       </c>
-      <c r="J54" s="14"/>
-      <c r="K54" s="14"/>
-      <c r="L54" s="17"/>
-      <c r="M54" s="17">
+      <c r="J54" s="11"/>
+      <c r="K54" s="11"/>
+      <c r="L54" s="14"/>
+      <c r="M54" s="14">
         <v>2013</v>
       </c>
-      <c r="N54" s="14"/>
-      <c r="O54" s="14"/>
-      <c r="P54" s="17"/>
-    </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A55" s="16">
+      <c r="N54" s="11"/>
+      <c r="O54" s="11"/>
+      <c r="P54" s="14"/>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A55" s="13">
         <v>2014</v>
       </c>
-      <c r="B55" s="14"/>
-      <c r="C55" s="14"/>
-      <c r="D55" s="17"/>
-      <c r="E55" s="17">
+      <c r="B55" s="11"/>
+      <c r="C55" s="11"/>
+      <c r="D55" s="14"/>
+      <c r="E55" s="14">
         <v>2014</v>
       </c>
-      <c r="F55" s="14"/>
-      <c r="G55" s="14"/>
-      <c r="H55" s="17"/>
-      <c r="I55" s="17">
+      <c r="F55" s="11"/>
+      <c r="G55" s="11"/>
+      <c r="H55" s="14"/>
+      <c r="I55" s="14">
         <v>2014</v>
       </c>
-      <c r="J55" s="14"/>
-      <c r="K55" s="14"/>
-      <c r="L55" s="17"/>
-      <c r="M55" s="17">
+      <c r="J55" s="11"/>
+      <c r="K55" s="11"/>
+      <c r="L55" s="14"/>
+      <c r="M55" s="14">
         <v>2014</v>
       </c>
-      <c r="N55" s="14"/>
-      <c r="O55" s="14"/>
-      <c r="P55" s="17"/>
-    </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A56" s="16">
+      <c r="N55" s="11"/>
+      <c r="O55" s="11"/>
+      <c r="P55" s="14"/>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A56" s="13">
         <v>2015</v>
       </c>
-      <c r="B56" s="14"/>
-      <c r="C56" s="14"/>
-      <c r="D56" s="17"/>
-      <c r="E56" s="17">
+      <c r="B56" s="11"/>
+      <c r="C56" s="11"/>
+      <c r="D56" s="14"/>
+      <c r="E56" s="14">
         <v>2015</v>
       </c>
-      <c r="F56" s="14"/>
-      <c r="G56" s="14"/>
-      <c r="H56" s="17"/>
-      <c r="I56" s="17">
+      <c r="F56" s="11"/>
+      <c r="G56" s="11"/>
+      <c r="H56" s="14"/>
+      <c r="I56" s="14">
         <v>2015</v>
       </c>
-      <c r="J56" s="14"/>
-      <c r="K56" s="14"/>
-      <c r="L56" s="17"/>
-      <c r="M56" s="17">
+      <c r="J56" s="11"/>
+      <c r="K56" s="11"/>
+      <c r="L56" s="14"/>
+      <c r="M56" s="14">
         <v>2015</v>
       </c>
-      <c r="N56" s="14"/>
-      <c r="O56" s="14"/>
-      <c r="P56" s="17"/>
-    </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A57" s="16">
+      <c r="N56" s="11"/>
+      <c r="O56" s="11"/>
+      <c r="P56" s="14"/>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A57" s="13">
         <v>2016</v>
       </c>
-      <c r="B57" s="14"/>
-      <c r="C57" s="14"/>
-      <c r="D57" s="17"/>
-      <c r="E57" s="17">
+      <c r="B57" s="11"/>
+      <c r="C57" s="11"/>
+      <c r="D57" s="14"/>
+      <c r="E57" s="14">
         <v>2016</v>
       </c>
-      <c r="F57" s="14"/>
-      <c r="G57" s="14"/>
-      <c r="H57" s="17"/>
-      <c r="I57" s="17">
+      <c r="F57" s="11"/>
+      <c r="G57" s="11"/>
+      <c r="H57" s="14"/>
+      <c r="I57" s="14">
         <v>2016</v>
       </c>
-      <c r="J57" s="14"/>
-      <c r="K57" s="14"/>
-      <c r="L57" s="17"/>
-      <c r="M57" s="17">
+      <c r="J57" s="11"/>
+      <c r="K57" s="11"/>
+      <c r="L57" s="14"/>
+      <c r="M57" s="14">
         <v>2016</v>
       </c>
-      <c r="N57" s="14"/>
-      <c r="O57" s="14"/>
-      <c r="P57" s="17"/>
-    </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A58" s="16">
+      <c r="N57" s="11"/>
+      <c r="O57" s="11"/>
+      <c r="P57" s="14"/>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A58" s="13">
         <v>2017</v>
       </c>
-      <c r="B58" s="14"/>
-      <c r="C58" s="14"/>
-      <c r="D58" s="17"/>
-      <c r="E58" s="17">
+      <c r="B58" s="11"/>
+      <c r="C58" s="11"/>
+      <c r="D58" s="14"/>
+      <c r="E58" s="14">
         <v>2017</v>
       </c>
-      <c r="F58" s="14"/>
-      <c r="G58" s="14"/>
-      <c r="H58" s="17"/>
-      <c r="I58" s="17">
+      <c r="F58" s="11"/>
+      <c r="G58" s="11"/>
+      <c r="H58" s="14"/>
+      <c r="I58" s="14">
         <v>2017</v>
       </c>
-      <c r="J58" s="14"/>
-      <c r="K58" s="14"/>
-      <c r="L58" s="17"/>
-      <c r="M58" s="17">
+      <c r="J58" s="11"/>
+      <c r="K58" s="11"/>
+      <c r="L58" s="14"/>
+      <c r="M58" s="14">
         <v>2017</v>
       </c>
-      <c r="N58" s="14"/>
-      <c r="O58" s="14"/>
-      <c r="P58" s="17"/>
-    </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A59" s="18">
+      <c r="N58" s="11"/>
+      <c r="O58" s="11"/>
+      <c r="P58" s="14"/>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A59" s="15">
         <v>2018</v>
       </c>
-      <c r="B59" s="19"/>
-      <c r="C59" s="19"/>
-      <c r="D59" s="15"/>
-      <c r="E59" s="15">
+      <c r="B59" s="16"/>
+      <c r="C59" s="16"/>
+      <c r="D59" s="12"/>
+      <c r="E59" s="12">
         <v>2018</v>
       </c>
-      <c r="F59" s="19"/>
-      <c r="G59" s="19"/>
-      <c r="H59" s="15"/>
-      <c r="I59" s="15">
+      <c r="F59" s="16"/>
+      <c r="G59" s="16"/>
+      <c r="H59" s="12"/>
+      <c r="I59" s="12">
         <v>2018</v>
       </c>
-      <c r="J59" s="19"/>
-      <c r="K59" s="19"/>
-      <c r="L59" s="15"/>
-      <c r="M59" s="15">
+      <c r="J59" s="16"/>
+      <c r="K59" s="16"/>
+      <c r="L59" s="12"/>
+      <c r="M59" s="12">
         <v>2018</v>
       </c>
-      <c r="N59" s="19"/>
-      <c r="O59" s="19"/>
-      <c r="P59" s="15"/>
+      <c r="N59" s="16"/>
+      <c r="O59" s="16"/>
+      <c r="P59" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="J20:L20"/>
+    <mergeCell ref="M20:M21"/>
+    <mergeCell ref="N20:P20"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="I20:I21"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="F1:H1"/>
     <mergeCell ref="J34:L34"/>
     <mergeCell ref="M34:M35"/>
     <mergeCell ref="N34:P34"/>
@@ -2170,22 +2383,6 @@
     <mergeCell ref="E34:E35"/>
     <mergeCell ref="F34:H34"/>
     <mergeCell ref="I34:I35"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="N1:P1"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="J20:L20"/>
-    <mergeCell ref="M20:M21"/>
-    <mergeCell ref="N20:P20"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="I20:I21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>